<commit_message>
Removed surplus models, Incorporated latest bug fixes from V3
</commit_message>
<xml_diff>
--- a/src/Chemistry/Chem4Word.Model/Resources/PeriodicTable.xlsx
+++ b/src/Chemistry/Chem4Word.Model/Resources/PeriodicTable.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\vso\chem4word\V.Next\Main\Chem4Word.Model\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\vso\chem4word\Version3\src\Chemistry\Chem4Word.Model\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PeriodicTable!$A$1:$M$141</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="448">
   <si>
     <t>Symbol</t>
   </si>
@@ -1330,12 +1330,48 @@
   </si>
   <si>
     <t>C# Property - Copy into PeriodicTable.cs</t>
+  </si>
+  <si>
+    <t>Uut</t>
+  </si>
+  <si>
+    <t>Ununtrium</t>
+  </si>
+  <si>
+    <t>Uuq</t>
+  </si>
+  <si>
+    <t>Ununquadium</t>
+  </si>
+  <si>
+    <t>Uup</t>
+  </si>
+  <si>
+    <t>Ununpentium</t>
+  </si>
+  <si>
+    <t>Uuh</t>
+  </si>
+  <si>
+    <t>Ununhexium</t>
+  </si>
+  <si>
+    <t>Uus</t>
+  </si>
+  <si>
+    <t>Ununseptium</t>
+  </si>
+  <si>
+    <t>Uuo</t>
+  </si>
+  <si>
+    <t>Ununoctium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1476,7 +1512,7 @@
       <name val="Helv"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1656,6 +1692,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1818,9 +1860,11 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2171,13 +2215,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q141"/>
+  <dimension ref="A1:Q147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q66" si="0">CONCATENATE("public Element ", A3, " { get; private set; } // ",B3," - Atomic Number ", C3)</f>
+        <f>CONCATENATE("public Element ", A3, " { get; private set; } // ",B3," - Atomic Number ", C3)</f>
         <v>public Element M { get; private set; } // Metal - Atomic Number 0</v>
       </c>
     </row>
@@ -2348,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="Q4" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A4, " { get; private set; } // ",B4," - Atomic Number ", C4)</f>
         <v>public Element R { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2381,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A5, " { get; private set; } // ",B5," - Atomic Number ", C5)</f>
         <v>public Element R1 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2414,7 +2458,7 @@
         <v>0</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A6, " { get; private set; } // ",B6," - Atomic Number ", C6)</f>
         <v>public Element R2 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2447,7 +2491,7 @@
         <v>0</v>
       </c>
       <c r="Q7" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A7, " { get; private set; } // ",B7," - Atomic Number ", C7)</f>
         <v>public Element R3 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2480,7 +2524,7 @@
         <v>0</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A8, " { get; private set; } // ",B8," - Atomic Number ", C8)</f>
         <v>public Element R4 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2513,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="Q9" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A9, " { get; private set; } // ",B9," - Atomic Number ", C9)</f>
         <v>public Element R5 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2546,7 +2590,7 @@
         <v>0</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A10, " { get; private set; } // ",B10," - Atomic Number ", C10)</f>
         <v>public Element R6 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2579,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A11, " { get; private set; } // ",B11," - Atomic Number ", C11)</f>
         <v>public Element R7 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2612,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A12, " { get; private set; } // ",B12," - Atomic Number ", C12)</f>
         <v>public Element R8 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2645,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A13, " { get; private set; } // ",B13," - Atomic Number ", C13)</f>
         <v>public Element R9 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2678,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A14, " { get; private set; } // ",B14," - Atomic Number ", C14)</f>
         <v>public Element R10 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2711,7 +2755,7 @@
         <v>0</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A15, " { get; private set; } // ",B15," - Atomic Number ", C15)</f>
         <v>public Element R11 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2744,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A16, " { get; private set; } // ",B16," - Atomic Number ", C16)</f>
         <v>public Element R12 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2777,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A17, " { get; private set; } // ",B17," - Atomic Number ", C17)</f>
         <v>public Element R13 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2810,7 +2854,7 @@
         <v>0</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A18, " { get; private set; } // ",B18," - Atomic Number ", C18)</f>
         <v>public Element R14 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2843,7 +2887,7 @@
         <v>0</v>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A19, " { get; private set; } // ",B19," - Atomic Number ", C19)</f>
         <v>public Element R15 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2876,7 +2920,7 @@
         <v>0</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A20, " { get; private set; } // ",B20," - Atomic Number ", C20)</f>
         <v>public Element R16 { get; private set; } // Residue - Atomic Number 0</v>
       </c>
     </row>
@@ -2909,7 +2953,7 @@
         <v>0</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A21, " { get; private set; } // ",B21," - Atomic Number ", C21)</f>
         <v>public Element X { get; private set; } // Halogen - Atomic Number 0</v>
       </c>
     </row>
@@ -2942,16 +2986,16 @@
         <v>2</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A22, " { get; private set; } // ",B22," - Atomic Number ", C22)</f>
         <v>public Element D { get; private set; } // Deuterium - Atomic Number 1</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2963,28 +3007,49 @@
         <v>12</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.31</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="H23">
         <v>1</v>
       </c>
       <c r="I23">
-        <v>3</v>
+        <v>1.0079400000000001</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
+        <v>399</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" si="0"/>
-        <v>public Element T { get; private set; } // Tritium - Atomic Number 1</v>
+        <f>CONCATENATE("public Element ", A23, " { get; private set; } // ",B23," - Atomic Number ", C23)</f>
+        <v>public Element H { get; private set; } // Hydrogen - Atomic Number 1</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2996,41 +3061,20 @@
         <v>12</v>
       </c>
       <c r="F24">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
       <c r="I24">
-        <v>1.0079400000000001</v>
-      </c>
-      <c r="J24" s="1">
-        <v>1</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="L24">
-        <v>1</v>
-      </c>
-      <c r="M24">
-        <v>1</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24" t="s">
-        <v>399</v>
+        <v>3</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" si="0"/>
-        <v>public Element H { get; private set; } // Hydrogen - Atomic Number 1</v>
+        <f>CONCATENATE("public Element ", A24, " { get; private set; } // ",B24," - Atomic Number ", C24)</f>
+        <v>public Element T { get; private set; } // Tritium - Atomic Number 1</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -3083,7 +3127,7 @@
         <v>400</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A25, " { get; private set; } // ",B25," - Atomic Number ", C25)</f>
         <v>public Element He { get; private set; } // Helium - Atomic Number 2</v>
       </c>
     </row>
@@ -3134,7 +3178,7 @@
         <v>401</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A26, " { get; private set; } // ",B26," - Atomic Number ", C26)</f>
         <v>public Element Li { get; private set; } // Lithium - Atomic Number 3</v>
       </c>
     </row>
@@ -3185,7 +3229,7 @@
         <v>402</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A27, " { get; private set; } // ",B27," - Atomic Number ", C27)</f>
         <v>public Element Be { get; private set; } // Beryllium - Atomic Number 4</v>
       </c>
     </row>
@@ -3239,7 +3283,7 @@
         <v>403</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A28, " { get; private set; } // ",B28," - Atomic Number ", C28)</f>
         <v>public Element B { get; private set; } // Boron - Atomic Number 5</v>
       </c>
     </row>
@@ -3293,7 +3337,7 @@
         <v>399</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A29, " { get; private set; } // ",B29," - Atomic Number ", C29)</f>
         <v>public Element C { get; private set; } // Carbon - Atomic Number 6</v>
       </c>
     </row>
@@ -3347,7 +3391,7 @@
         <v>399</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A30, " { get; private set; } // ",B30," - Atomic Number ", C30)</f>
         <v>public Element N { get; private set; } // Nitrogen - Atomic Number 7</v>
       </c>
     </row>
@@ -3401,7 +3445,7 @@
         <v>399</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A31, " { get; private set; } // ",B31," - Atomic Number ", C31)</f>
         <v>public Element O { get; private set; } // Oxygen - Atomic Number 8</v>
       </c>
     </row>
@@ -3455,7 +3499,7 @@
         <v>404</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A32, " { get; private set; } // ",B32," - Atomic Number ", C32)</f>
         <v>public Element F { get; private set; } // Fluorine - Atomic Number 9</v>
       </c>
     </row>
@@ -3506,7 +3550,7 @@
         <v>400</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A33, " { get; private set; } // ",B33," - Atomic Number ", C33)</f>
         <v>public Element Ne { get; private set; } // Neon - Atomic Number 10</v>
       </c>
     </row>
@@ -3557,7 +3601,7 @@
         <v>401</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A34, " { get; private set; } // ",B34," - Atomic Number ", C34)</f>
         <v>public Element Na { get; private set; } // Sodium - Atomic Number 11</v>
       </c>
     </row>
@@ -3608,7 +3652,7 @@
         <v>402</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A35, " { get; private set; } // ",B35," - Atomic Number ", C35)</f>
         <v>public Element Mg { get; private set; } // Magnesium - Atomic Number 12</v>
       </c>
     </row>
@@ -3659,7 +3703,7 @@
         <v>405</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A36, " { get; private set; } // ",B36," - Atomic Number ", C36)</f>
         <v>public Element Al { get; private set; } // Aluminum - Atomic Number 13</v>
       </c>
     </row>
@@ -3710,7 +3754,7 @@
         <v>403</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A37, " { get; private set; } // ",B37," - Atomic Number ", C37)</f>
         <v>public Element Si { get; private set; } // Silicon - Atomic Number 14</v>
       </c>
     </row>
@@ -3761,7 +3805,7 @@
         <v>399</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A38, " { get; private set; } // ",B38," - Atomic Number ", C38)</f>
         <v>public Element P { get; private set; } // Phosphorus - Atomic Number 15</v>
       </c>
     </row>
@@ -3812,7 +3856,7 @@
         <v>399</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A39, " { get; private set; } // ",B39," - Atomic Number ", C39)</f>
         <v>public Element S { get; private set; } // Sulfur - Atomic Number 16</v>
       </c>
     </row>
@@ -3866,7 +3910,7 @@
         <v>404</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A40, " { get; private set; } // ",B40," - Atomic Number ", C40)</f>
         <v>public Element Cl { get; private set; } // Chlorine - Atomic Number 17</v>
       </c>
     </row>
@@ -3917,7 +3961,7 @@
         <v>400</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A41, " { get; private set; } // ",B41," - Atomic Number ", C41)</f>
         <v>public Element Ar { get; private set; } // Argon - Atomic Number 18</v>
       </c>
     </row>
@@ -3968,7 +4012,7 @@
         <v>401</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A42, " { get; private set; } // ",B42," - Atomic Number ", C42)</f>
         <v>public Element K { get; private set; } // Potassium - Atomic Number 19</v>
       </c>
     </row>
@@ -4019,7 +4063,7 @@
         <v>402</v>
       </c>
       <c r="Q43" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A43, " { get; private set; } // ",B43," - Atomic Number ", C43)</f>
         <v>public Element Ca { get; private set; } // Calcium - Atomic Number 20</v>
       </c>
     </row>
@@ -4070,7 +4114,7 @@
         <v>406</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A44, " { get; private set; } // ",B44," - Atomic Number ", C44)</f>
         <v>public Element Sc { get; private set; } // Scandium - Atomic Number 21</v>
       </c>
     </row>
@@ -4121,7 +4165,7 @@
         <v>406</v>
       </c>
       <c r="Q45" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A45, " { get; private set; } // ",B45," - Atomic Number ", C45)</f>
         <v>public Element Ti { get; private set; } // Titanium - Atomic Number 22</v>
       </c>
     </row>
@@ -4172,7 +4216,7 @@
         <v>406</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A46, " { get; private set; } // ",B46," - Atomic Number ", C46)</f>
         <v>public Element V { get; private set; } // Vanadium - Atomic Number 23</v>
       </c>
     </row>
@@ -4223,7 +4267,7 @@
         <v>406</v>
       </c>
       <c r="Q47" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A47, " { get; private set; } // ",B47," - Atomic Number ", C47)</f>
         <v>public Element Cr { get; private set; } // Chromium - Atomic Number 24</v>
       </c>
     </row>
@@ -4274,7 +4318,7 @@
         <v>406</v>
       </c>
       <c r="Q48" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A48, " { get; private set; } // ",B48," - Atomic Number ", C48)</f>
         <v>public Element Mn { get; private set; } // Manganese - Atomic Number 25</v>
       </c>
     </row>
@@ -4325,7 +4369,7 @@
         <v>406</v>
       </c>
       <c r="Q49" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A49, " { get; private set; } // ",B49," - Atomic Number ", C49)</f>
         <v>public Element Fe { get; private set; } // Iron - Atomic Number 26</v>
       </c>
     </row>
@@ -4376,7 +4420,7 @@
         <v>406</v>
       </c>
       <c r="Q50" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A50, " { get; private set; } // ",B50," - Atomic Number ", C50)</f>
         <v>public Element Co { get; private set; } // Cobalt - Atomic Number 27</v>
       </c>
     </row>
@@ -4427,7 +4471,7 @@
         <v>406</v>
       </c>
       <c r="Q51" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A51, " { get; private set; } // ",B51," - Atomic Number ", C51)</f>
         <v>public Element Ni { get; private set; } // Nickel - Atomic Number 28</v>
       </c>
     </row>
@@ -4478,7 +4522,7 @@
         <v>406</v>
       </c>
       <c r="Q52" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A52, " { get; private set; } // ",B52," - Atomic Number ", C52)</f>
         <v>public Element Cu { get; private set; } // Copper - Atomic Number 29</v>
       </c>
     </row>
@@ -4529,7 +4573,7 @@
         <v>406</v>
       </c>
       <c r="Q53" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A53, " { get; private set; } // ",B53," - Atomic Number ", C53)</f>
         <v>public Element Zn { get; private set; } // Zinc - Atomic Number 30</v>
       </c>
     </row>
@@ -4580,7 +4624,7 @@
         <v>405</v>
       </c>
       <c r="Q54" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A54, " { get; private set; } // ",B54," - Atomic Number ", C54)</f>
         <v>public Element Ga { get; private set; } // Gallium - Atomic Number 31</v>
       </c>
     </row>
@@ -4631,7 +4675,7 @@
         <v>403</v>
       </c>
       <c r="Q55" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A55, " { get; private set; } // ",B55," - Atomic Number ", C55)</f>
         <v>public Element Ge { get; private set; } // Germanium - Atomic Number 32</v>
       </c>
     </row>
@@ -4682,7 +4726,7 @@
         <v>403</v>
       </c>
       <c r="Q56" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A56, " { get; private set; } // ",B56," - Atomic Number ", C56)</f>
         <v>public Element As { get; private set; } // Arsenic - Atomic Number 33</v>
       </c>
     </row>
@@ -4733,7 +4777,7 @@
         <v>399</v>
       </c>
       <c r="Q57" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A57, " { get; private set; } // ",B57," - Atomic Number ", C57)</f>
         <v>public Element Se { get; private set; } // Selenium - Atomic Number 34</v>
       </c>
     </row>
@@ -4784,7 +4828,7 @@
         <v>404</v>
       </c>
       <c r="Q58" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A58, " { get; private set; } // ",B58," - Atomic Number ", C58)</f>
         <v>public Element Br { get; private set; } // Bromine - Atomic Number 35</v>
       </c>
     </row>
@@ -4835,7 +4879,7 @@
         <v>400</v>
       </c>
       <c r="Q59" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A59, " { get; private set; } // ",B59," - Atomic Number ", C59)</f>
         <v>public Element Kr { get; private set; } // Krypton - Atomic Number 36</v>
       </c>
     </row>
@@ -4886,7 +4930,7 @@
         <v>401</v>
       </c>
       <c r="Q60" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A60, " { get; private set; } // ",B60," - Atomic Number ", C60)</f>
         <v>public Element Rb { get; private set; } // Rubidium - Atomic Number 37</v>
       </c>
     </row>
@@ -4937,7 +4981,7 @@
         <v>402</v>
       </c>
       <c r="Q61" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A61, " { get; private set; } // ",B61," - Atomic Number ", C61)</f>
         <v>public Element Sr { get; private set; } // Strontium - Atomic Number 38</v>
       </c>
     </row>
@@ -4988,7 +5032,7 @@
         <v>406</v>
       </c>
       <c r="Q62" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A62, " { get; private set; } // ",B62," - Atomic Number ", C62)</f>
         <v>public Element Y { get; private set; } // Yttrium - Atomic Number 39</v>
       </c>
     </row>
@@ -5039,7 +5083,7 @@
         <v>406</v>
       </c>
       <c r="Q63" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A63, " { get; private set; } // ",B63," - Atomic Number ", C63)</f>
         <v>public Element Zr { get; private set; } // Zirconium - Atomic Number 40</v>
       </c>
     </row>
@@ -5090,7 +5134,7 @@
         <v>406</v>
       </c>
       <c r="Q64" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A64, " { get; private set; } // ",B64," - Atomic Number ", C64)</f>
         <v>public Element Nb { get; private set; } // Niobium - Atomic Number 41</v>
       </c>
     </row>
@@ -5141,7 +5185,7 @@
         <v>406</v>
       </c>
       <c r="Q65" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A65, " { get; private set; } // ",B65," - Atomic Number ", C65)</f>
         <v>public Element Mo { get; private set; } // Molybdenum - Atomic Number 42</v>
       </c>
     </row>
@@ -5192,7 +5236,7 @@
         <v>406</v>
       </c>
       <c r="Q66" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("public Element ", A66, " { get; private set; } // ",B66," - Atomic Number ", C66)</f>
         <v>public Element Tc { get; private set; } // Technetium - Atomic Number 43</v>
       </c>
     </row>
@@ -5243,7 +5287,7 @@
         <v>406</v>
       </c>
       <c r="Q67" t="str">
-        <f t="shared" ref="Q67:Q130" si="1">CONCATENATE("public Element ", A67, " { get; private set; } // ",B67," - Atomic Number ", C67)</f>
+        <f>CONCATENATE("public Element ", A67, " { get; private set; } // ",B67," - Atomic Number ", C67)</f>
         <v>public Element Ru { get; private set; } // Ruthenium - Atomic Number 44</v>
       </c>
     </row>
@@ -5294,7 +5338,7 @@
         <v>406</v>
       </c>
       <c r="Q68" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A68, " { get; private set; } // ",B68," - Atomic Number ", C68)</f>
         <v>public Element Rh { get; private set; } // Rhodium - Atomic Number 45</v>
       </c>
     </row>
@@ -5345,7 +5389,7 @@
         <v>406</v>
       </c>
       <c r="Q69" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A69, " { get; private set; } // ",B69," - Atomic Number ", C69)</f>
         <v>public Element Pd { get; private set; } // Palladium - Atomic Number 46</v>
       </c>
     </row>
@@ -5396,7 +5440,7 @@
         <v>406</v>
       </c>
       <c r="Q70" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A70, " { get; private set; } // ",B70," - Atomic Number ", C70)</f>
         <v>public Element Ag { get; private set; } // Silver - Atomic Number 47</v>
       </c>
     </row>
@@ -5447,7 +5491,7 @@
         <v>406</v>
       </c>
       <c r="Q71" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A71, " { get; private set; } // ",B71," - Atomic Number ", C71)</f>
         <v>public Element Cd { get; private set; } // Cadmium - Atomic Number 48</v>
       </c>
     </row>
@@ -5498,7 +5542,7 @@
         <v>405</v>
       </c>
       <c r="Q72" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A72, " { get; private set; } // ",B72," - Atomic Number ", C72)</f>
         <v>public Element In { get; private set; } // Indium - Atomic Number 49</v>
       </c>
     </row>
@@ -5549,7 +5593,7 @@
         <v>405</v>
       </c>
       <c r="Q73" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A73, " { get; private set; } // ",B73," - Atomic Number ", C73)</f>
         <v>public Element Sn { get; private set; } // Tin - Atomic Number 50</v>
       </c>
     </row>
@@ -5600,7 +5644,7 @@
         <v>403</v>
       </c>
       <c r="Q74" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A74, " { get; private set; } // ",B74," - Atomic Number ", C74)</f>
         <v>public Element Sb { get; private set; } // Antimony - Atomic Number 51</v>
       </c>
     </row>
@@ -5651,7 +5695,7 @@
         <v>403</v>
       </c>
       <c r="Q75" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A75, " { get; private set; } // ",B75," - Atomic Number ", C75)</f>
         <v>public Element Te { get; private set; } // Tellurium - Atomic Number 52</v>
       </c>
     </row>
@@ -5702,7 +5746,7 @@
         <v>404</v>
       </c>
       <c r="Q76" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A76, " { get; private set; } // ",B76," - Atomic Number ", C76)</f>
         <v>public Element I { get; private set; } // Iodine - Atomic Number 53</v>
       </c>
     </row>
@@ -5753,7 +5797,7 @@
         <v>400</v>
       </c>
       <c r="Q77" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A77, " { get; private set; } // ",B77," - Atomic Number ", C77)</f>
         <v>public Element Xe { get; private set; } // Xenon - Atomic Number 54</v>
       </c>
     </row>
@@ -5804,7 +5848,7 @@
         <v>401</v>
       </c>
       <c r="Q78" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A78, " { get; private set; } // ",B78," - Atomic Number ", C78)</f>
         <v>public Element Cs { get; private set; } // Cesium - Atomic Number 55</v>
       </c>
     </row>
@@ -5855,7 +5899,7 @@
         <v>402</v>
       </c>
       <c r="Q79" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A79, " { get; private set; } // ",B79," - Atomic Number ", C79)</f>
         <v>public Element Ba { get; private set; } // Barium - Atomic Number 56</v>
       </c>
     </row>
@@ -5906,7 +5950,7 @@
         <v>407</v>
       </c>
       <c r="Q80" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A80, " { get; private set; } // ",B80," - Atomic Number ", C80)</f>
         <v>public Element La { get; private set; } // Lanthanum - Atomic Number 57</v>
       </c>
     </row>
@@ -5957,7 +6001,7 @@
         <v>407</v>
       </c>
       <c r="Q81" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A81, " { get; private set; } // ",B81," - Atomic Number ", C81)</f>
         <v>public Element Ce { get; private set; } // Cerium - Atomic Number 58</v>
       </c>
     </row>
@@ -6008,7 +6052,7 @@
         <v>407</v>
       </c>
       <c r="Q82" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A82, " { get; private set; } // ",B82," - Atomic Number ", C82)</f>
         <v>public Element Pr { get; private set; } // Praseodymium - Atomic Number 59</v>
       </c>
     </row>
@@ -6059,7 +6103,7 @@
         <v>407</v>
       </c>
       <c r="Q83" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A83, " { get; private set; } // ",B83," - Atomic Number ", C83)</f>
         <v>public Element Nd { get; private set; } // Neodymium - Atomic Number 60</v>
       </c>
     </row>
@@ -6110,7 +6154,7 @@
         <v>407</v>
       </c>
       <c r="Q84" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A84, " { get; private set; } // ",B84," - Atomic Number ", C84)</f>
         <v>public Element Pm { get; private set; } // Promethium - Atomic Number 61</v>
       </c>
     </row>
@@ -6161,7 +6205,7 @@
         <v>407</v>
       </c>
       <c r="Q85" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A85, " { get; private set; } // ",B85," - Atomic Number ", C85)</f>
         <v>public Element Sm { get; private set; } // Samarium - Atomic Number 62</v>
       </c>
     </row>
@@ -6212,7 +6256,7 @@
         <v>407</v>
       </c>
       <c r="Q86" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A86, " { get; private set; } // ",B86," - Atomic Number ", C86)</f>
         <v>public Element Eu { get; private set; } // Europium - Atomic Number 63</v>
       </c>
     </row>
@@ -6263,7 +6307,7 @@
         <v>407</v>
       </c>
       <c r="Q87" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A87, " { get; private set; } // ",B87," - Atomic Number ", C87)</f>
         <v>public Element Gd { get; private set; } // Gadolinium - Atomic Number 64</v>
       </c>
     </row>
@@ -6314,7 +6358,7 @@
         <v>407</v>
       </c>
       <c r="Q88" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A88, " { get; private set; } // ",B88," - Atomic Number ", C88)</f>
         <v>public Element Tb { get; private set; } // Terbium - Atomic Number 65</v>
       </c>
     </row>
@@ -6365,7 +6409,7 @@
         <v>407</v>
       </c>
       <c r="Q89" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A89, " { get; private set; } // ",B89," - Atomic Number ", C89)</f>
         <v>public Element Dy { get; private set; } // Dysprosium - Atomic Number 66</v>
       </c>
     </row>
@@ -6416,7 +6460,7 @@
         <v>407</v>
       </c>
       <c r="Q90" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A90, " { get; private set; } // ",B90," - Atomic Number ", C90)</f>
         <v>public Element Ho { get; private set; } // Holmium - Atomic Number 67</v>
       </c>
     </row>
@@ -6467,7 +6511,7 @@
         <v>407</v>
       </c>
       <c r="Q91" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A91, " { get; private set; } // ",B91," - Atomic Number ", C91)</f>
         <v>public Element Er { get; private set; } // Erbium - Atomic Number 68</v>
       </c>
     </row>
@@ -6518,7 +6562,7 @@
         <v>407</v>
       </c>
       <c r="Q92" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A92, " { get; private set; } // ",B92," - Atomic Number ", C92)</f>
         <v>public Element Tm { get; private set; } // Thulium - Atomic Number 69</v>
       </c>
     </row>
@@ -6569,7 +6613,7 @@
         <v>407</v>
       </c>
       <c r="Q93" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A93, " { get; private set; } // ",B93," - Atomic Number ", C93)</f>
         <v>public Element Yb { get; private set; } // Ytterbium - Atomic Number 70</v>
       </c>
     </row>
@@ -6620,7 +6664,7 @@
         <v>406</v>
       </c>
       <c r="Q94" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A94, " { get; private set; } // ",B94," - Atomic Number ", C94)</f>
         <v>public Element Lu { get; private set; } // Lutetium - Atomic Number 71</v>
       </c>
     </row>
@@ -6671,7 +6715,7 @@
         <v>406</v>
       </c>
       <c r="Q95" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A95, " { get; private set; } // ",B95," - Atomic Number ", C95)</f>
         <v>public Element Hf { get; private set; } // Hafnium - Atomic Number 72</v>
       </c>
     </row>
@@ -6722,7 +6766,7 @@
         <v>406</v>
       </c>
       <c r="Q96" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A96, " { get; private set; } // ",B96," - Atomic Number ", C96)</f>
         <v>public Element Ta { get; private set; } // Tantalum - Atomic Number 73</v>
       </c>
     </row>
@@ -6773,7 +6817,7 @@
         <v>406</v>
       </c>
       <c r="Q97" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A97, " { get; private set; } // ",B97," - Atomic Number ", C97)</f>
         <v>public Element W { get; private set; } // Tungsten - Atomic Number 74</v>
       </c>
     </row>
@@ -6824,7 +6868,7 @@
         <v>406</v>
       </c>
       <c r="Q98" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A98, " { get; private set; } // ",B98," - Atomic Number ", C98)</f>
         <v>public Element Re { get; private set; } // Rhenium - Atomic Number 75</v>
       </c>
     </row>
@@ -6875,7 +6919,7 @@
         <v>406</v>
       </c>
       <c r="Q99" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A99, " { get; private set; } // ",B99," - Atomic Number ", C99)</f>
         <v>public Element Os { get; private set; } // Osmium - Atomic Number 76</v>
       </c>
     </row>
@@ -6926,7 +6970,7 @@
         <v>406</v>
       </c>
       <c r="Q100" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A100, " { get; private set; } // ",B100," - Atomic Number ", C100)</f>
         <v>public Element Ir { get; private set; } // Iridium - Atomic Number 77</v>
       </c>
     </row>
@@ -6977,7 +7021,7 @@
         <v>406</v>
       </c>
       <c r="Q101" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A101, " { get; private set; } // ",B101," - Atomic Number ", C101)</f>
         <v>public Element Pt { get; private set; } // Platinum - Atomic Number 78</v>
       </c>
     </row>
@@ -7028,7 +7072,7 @@
         <v>406</v>
       </c>
       <c r="Q102" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A102, " { get; private set; } // ",B102," - Atomic Number ", C102)</f>
         <v>public Element Au { get; private set; } // Gold - Atomic Number 79</v>
       </c>
     </row>
@@ -7079,7 +7123,7 @@
         <v>406</v>
       </c>
       <c r="Q103" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A103, " { get; private set; } // ",B103," - Atomic Number ", C103)</f>
         <v>public Element Hg { get; private set; } // Mercury - Atomic Number 80</v>
       </c>
     </row>
@@ -7130,7 +7174,7 @@
         <v>405</v>
       </c>
       <c r="Q104" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A104, " { get; private set; } // ",B104," - Atomic Number ", C104)</f>
         <v>public Element Tl { get; private set; } // Thallium - Atomic Number 81</v>
       </c>
     </row>
@@ -7181,7 +7225,7 @@
         <v>405</v>
       </c>
       <c r="Q105" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A105, " { get; private set; } // ",B105," - Atomic Number ", C105)</f>
         <v>public Element Pb { get; private set; } // Lead - Atomic Number 82</v>
       </c>
     </row>
@@ -7232,7 +7276,7 @@
         <v>405</v>
       </c>
       <c r="Q106" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A106, " { get; private set; } // ",B106," - Atomic Number ", C106)</f>
         <v>public Element Bi { get; private set; } // Bismuth - Atomic Number 83</v>
       </c>
     </row>
@@ -7283,7 +7327,7 @@
         <v>403</v>
       </c>
       <c r="Q107" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A107, " { get; private set; } // ",B107," - Atomic Number ", C107)</f>
         <v>public Element Po { get; private set; } // Polonium - Atomic Number 84</v>
       </c>
     </row>
@@ -7334,7 +7378,7 @@
         <v>404</v>
       </c>
       <c r="Q108" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A108, " { get; private set; } // ",B108," - Atomic Number ", C108)</f>
         <v>public Element At { get; private set; } // Astatine - Atomic Number 85</v>
       </c>
     </row>
@@ -7385,7 +7429,7 @@
         <v>400</v>
       </c>
       <c r="Q109" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A109, " { get; private set; } // ",B109," - Atomic Number ", C109)</f>
         <v>public Element Rn { get; private set; } // Radon - Atomic Number 86</v>
       </c>
     </row>
@@ -7436,7 +7480,7 @@
         <v>401</v>
       </c>
       <c r="Q110" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A110, " { get; private set; } // ",B110," - Atomic Number ", C110)</f>
         <v>public Element Fr { get; private set; } // Francium - Atomic Number 87</v>
       </c>
     </row>
@@ -7487,7 +7531,7 @@
         <v>402</v>
       </c>
       <c r="Q111" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A111, " { get; private set; } // ",B111," - Atomic Number ", C111)</f>
         <v>public Element Ra { get; private set; } // Radium - Atomic Number 88</v>
       </c>
     </row>
@@ -7535,7 +7579,7 @@
         <v>408</v>
       </c>
       <c r="Q112" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A112, " { get; private set; } // ",B112," - Atomic Number ", C112)</f>
         <v>public Element Ac { get; private set; } // Actinium - Atomic Number 89</v>
       </c>
     </row>
@@ -7586,7 +7630,7 @@
         <v>408</v>
       </c>
       <c r="Q113" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A113, " { get; private set; } // ",B113," - Atomic Number ", C113)</f>
         <v>public Element Th { get; private set; } // Thorium - Atomic Number 90</v>
       </c>
     </row>
@@ -7637,7 +7681,7 @@
         <v>408</v>
       </c>
       <c r="Q114" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A114, " { get; private set; } // ",B114," - Atomic Number ", C114)</f>
         <v>public Element Pa { get; private set; } // Protactinium - Atomic Number 91</v>
       </c>
     </row>
@@ -7688,7 +7732,7 @@
         <v>408</v>
       </c>
       <c r="Q115" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A115, " { get; private set; } // ",B115," - Atomic Number ", C115)</f>
         <v>public Element U { get; private set; } // Uranium - Atomic Number 92</v>
       </c>
     </row>
@@ -7739,7 +7783,7 @@
         <v>408</v>
       </c>
       <c r="Q116" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A116, " { get; private set; } // ",B116," - Atomic Number ", C116)</f>
         <v>public Element Np { get; private set; } // Neptunium - Atomic Number 93</v>
       </c>
     </row>
@@ -7790,7 +7834,7 @@
         <v>408</v>
       </c>
       <c r="Q117" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A117, " { get; private set; } // ",B117," - Atomic Number ", C117)</f>
         <v>public Element Pu { get; private set; } // Plutonium - Atomic Number 94</v>
       </c>
     </row>
@@ -7841,7 +7885,7 @@
         <v>408</v>
       </c>
       <c r="Q118" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A118, " { get; private set; } // ",B118," - Atomic Number ", C118)</f>
         <v>public Element Am { get; private set; } // Americium - Atomic Number 95</v>
       </c>
     </row>
@@ -7892,7 +7936,7 @@
         <v>408</v>
       </c>
       <c r="Q119" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A119, " { get; private set; } // ",B119," - Atomic Number ", C119)</f>
         <v>public Element Cm { get; private set; } // Curium - Atomic Number 96</v>
       </c>
     </row>
@@ -7943,7 +7987,7 @@
         <v>408</v>
       </c>
       <c r="Q120" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A120, " { get; private set; } // ",B120," - Atomic Number ", C120)</f>
         <v>public Element Bk { get; private set; } // Berkelium - Atomic Number 97</v>
       </c>
     </row>
@@ -7991,7 +8035,7 @@
         <v>408</v>
       </c>
       <c r="Q121" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A121, " { get; private set; } // ",B121," - Atomic Number ", C121)</f>
         <v>public Element Cf { get; private set; } // Californium - Atomic Number 98</v>
       </c>
     </row>
@@ -8039,7 +8083,7 @@
         <v>408</v>
       </c>
       <c r="Q122" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A122, " { get; private set; } // ",B122," - Atomic Number ", C122)</f>
         <v>public Element Es { get; private set; } // Einsteinium - Atomic Number 99</v>
       </c>
     </row>
@@ -8087,7 +8131,7 @@
         <v>408</v>
       </c>
       <c r="Q123" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A123, " { get; private set; } // ",B123," - Atomic Number ", C123)</f>
         <v>public Element Fm { get; private set; } // Fermium - Atomic Number 100</v>
       </c>
     </row>
@@ -8138,7 +8182,7 @@
         <v>408</v>
       </c>
       <c r="Q124" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A124, " { get; private set; } // ",B124," - Atomic Number ", C124)</f>
         <v>public Element Md { get; private set; } // Mendelevium - Atomic Number 101</v>
       </c>
     </row>
@@ -8186,7 +8230,7 @@
         <v>408</v>
       </c>
       <c r="Q125" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A125, " { get; private set; } // ",B125," - Atomic Number ", C125)</f>
         <v>public Element No { get; private set; } // Nobelium - Atomic Number 102</v>
       </c>
     </row>
@@ -8237,7 +8281,7 @@
         <v>406</v>
       </c>
       <c r="Q126" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A126, " { get; private set; } // ",B126," - Atomic Number ", C126)</f>
         <v>public Element Lr { get; private set; } // Lawrencium - Atomic Number 103</v>
       </c>
     </row>
@@ -8285,7 +8329,7 @@
         <v>406</v>
       </c>
       <c r="Q127" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A127, " { get; private set; } // ",B127," - Atomic Number ", C127)</f>
         <v>public Element Rf { get; private set; } // Rutherfordium - Atomic Number 104</v>
       </c>
     </row>
@@ -8333,7 +8377,7 @@
         <v>406</v>
       </c>
       <c r="Q128" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A128, " { get; private set; } // ",B128," - Atomic Number ", C128)</f>
         <v>public Element Db { get; private set; } // Dubnium - Atomic Number 105</v>
       </c>
     </row>
@@ -8381,7 +8425,7 @@
         <v>406</v>
       </c>
       <c r="Q129" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A129, " { get; private set; } // ",B129," - Atomic Number ", C129)</f>
         <v>public Element Sg { get; private set; } // Seaborgium - Atomic Number 106</v>
       </c>
     </row>
@@ -8426,7 +8470,7 @@
         <v>406</v>
       </c>
       <c r="Q130" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("public Element ", A130, " { get; private set; } // ",B130," - Atomic Number ", C130)</f>
         <v>public Element Bh { get; private set; } // Bohrium - Atomic Number 107</v>
       </c>
     </row>
@@ -8471,7 +8515,7 @@
         <v>406</v>
       </c>
       <c r="Q131" t="str">
-        <f t="shared" ref="Q131:Q141" si="2">CONCATENATE("public Element ", A131, " { get; private set; } // ",B131," - Atomic Number ", C131)</f>
+        <f>CONCATENATE("public Element ", A131, " { get; private set; } // ",B131," - Atomic Number ", C131)</f>
         <v>public Element Hs { get; private set; } // Hassium - Atomic Number 108</v>
       </c>
     </row>
@@ -8516,7 +8560,7 @@
         <v>406</v>
       </c>
       <c r="Q132" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("public Element ", A132, " { get; private set; } // ",B132," - Atomic Number ", C132)</f>
         <v>public Element Mt { get; private set; } // Meitnerium - Atomic Number 109</v>
       </c>
     </row>
@@ -8561,7 +8605,7 @@
         <v>406</v>
       </c>
       <c r="Q133" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("public Element ", A133, " { get; private set; } // ",B133," - Atomic Number ", C133)</f>
         <v>public Element Ds { get; private set; } // Darmstadtium - Atomic Number 110</v>
       </c>
     </row>
@@ -8603,7 +8647,7 @@
         <v>406</v>
       </c>
       <c r="Q134" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("public Element ", A134, " { get; private set; } // ",B134," - Atomic Number ", C134)</f>
         <v>public Element Rg { get; private set; } // Roentgenium - Atomic Number 111</v>
       </c>
     </row>
@@ -8645,7 +8689,7 @@
         <v>406</v>
       </c>
       <c r="Q135" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("public Element ", A135, " { get; private set; } // ",B135," - Atomic Number ", C135)</f>
         <v>public Element Cn { get; private set; } // Copernicium - Atomic Number 112</v>
       </c>
     </row>
@@ -8687,61 +8731,63 @@
         <v>409</v>
       </c>
       <c r="Q136" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("public Element ", A136, " { get; private set; } // ",B136," - Atomic Number ", C136)</f>
         <v>public Element Nh { get; private set; } // Nihonium - Atomic Number 113</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>397</v>
-      </c>
-      <c r="B137" t="s">
-        <v>395</v>
-      </c>
-      <c r="C137">
-        <v>114</v>
-      </c>
-      <c r="D137" t="b">
-        <v>0</v>
-      </c>
-      <c r="E137" t="s">
+    <row r="137" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C137" s="3">
+        <v>113</v>
+      </c>
+      <c r="D137" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E137" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="F137">
-        <v>0</v>
-      </c>
-      <c r="G137">
-        <v>0</v>
-      </c>
-      <c r="H137">
-        <v>0</v>
-      </c>
-      <c r="I137">
-        <v>0</v>
-      </c>
-      <c r="N137">
+      <c r="F137" s="3">
+        <v>0</v>
+      </c>
+      <c r="G137" s="3">
+        <v>0</v>
+      </c>
+      <c r="H137" s="3">
+        <v>0</v>
+      </c>
+      <c r="I137" s="3">
+        <v>0</v>
+      </c>
+      <c r="J137" s="2"/>
+      <c r="K137" s="2"/>
+      <c r="N137" s="3">
         <v>6</v>
       </c>
-      <c r="O137">
-        <v>13</v>
-      </c>
-      <c r="P137" t="s">
+      <c r="O137" s="3">
+        <v>12</v>
+      </c>
+      <c r="P137" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="Q137" t="str">
-        <f t="shared" si="2"/>
-        <v>public Element Fl { get; private set; } // Flerovium - Atomic Number 114</v>
+      <c r="Q137" s="3" t="str">
+        <f>CONCATENATE("public Element ", A137, " { get; private set; } // ",B137," - Atomic Number ", C137)</f>
+        <v>public Element Uut { get; private set; } // Ununtrium - Atomic Number 113</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>427</v>
+        <v>397</v>
       </c>
       <c r="B138" t="s">
-        <v>431</v>
+        <v>395</v>
       </c>
       <c r="C138">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D138" t="b">
         <v>0</v>
@@ -8765,67 +8811,69 @@
         <v>6</v>
       </c>
       <c r="O138">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P138" t="s">
         <v>409</v>
       </c>
       <c r="Q138" t="str">
-        <f t="shared" si="2"/>
-        <v>public Element Mc { get; private set; } // Moscovium - Atomic Number 115</v>
-      </c>
-    </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>398</v>
-      </c>
-      <c r="B139" t="s">
-        <v>396</v>
-      </c>
-      <c r="C139">
-        <v>116</v>
-      </c>
-      <c r="D139" t="b">
-        <v>0</v>
-      </c>
-      <c r="E139" t="s">
+        <f>CONCATENATE("public Element ", A138, " { get; private set; } // ",B138," - Atomic Number ", C138)</f>
+        <v>public Element Fl { get; private set; } // Flerovium - Atomic Number 114</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="C139" s="3">
+        <v>114</v>
+      </c>
+      <c r="D139" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E139" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="F139">
-        <v>0</v>
-      </c>
-      <c r="G139">
-        <v>0</v>
-      </c>
-      <c r="H139">
-        <v>0</v>
-      </c>
-      <c r="I139">
-        <v>0</v>
-      </c>
-      <c r="N139">
+      <c r="F139" s="3">
+        <v>0</v>
+      </c>
+      <c r="G139" s="3">
+        <v>0</v>
+      </c>
+      <c r="H139" s="3">
+        <v>0</v>
+      </c>
+      <c r="I139" s="3">
+        <v>0</v>
+      </c>
+      <c r="J139" s="2"/>
+      <c r="K139" s="2"/>
+      <c r="N139" s="3">
         <v>6</v>
       </c>
-      <c r="O139">
-        <v>15</v>
-      </c>
-      <c r="P139" t="s">
+      <c r="O139" s="3">
+        <v>13</v>
+      </c>
+      <c r="P139" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="Q139" t="str">
-        <f t="shared" si="2"/>
-        <v>public Element Lv { get; private set; } // Livermorium - Atomic Number 116</v>
+      <c r="Q139" s="3" t="str">
+        <f>CONCATENATE("public Element ", A139, " { get; private set; } // ",B139," - Atomic Number ", C139)</f>
+        <v>public Element Uuq { get; private set; } // Ununquadium - Atomic Number 114</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B140" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C140">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D140" t="b">
         <v>0</v>
@@ -8849,62 +8897,323 @@
         <v>6</v>
       </c>
       <c r="O140">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P140" t="s">
         <v>409</v>
       </c>
       <c r="Q140" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("public Element ", A140, " { get; private set; } // ",B140," - Atomic Number ", C140)</f>
+        <v>public Element Mc { get; private set; } // Moscovium - Atomic Number 115</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="C141" s="3">
+        <v>115</v>
+      </c>
+      <c r="D141" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="F141" s="3">
+        <v>0</v>
+      </c>
+      <c r="G141" s="3">
+        <v>0</v>
+      </c>
+      <c r="H141" s="3">
+        <v>0</v>
+      </c>
+      <c r="I141" s="3">
+        <v>0</v>
+      </c>
+      <c r="J141" s="2"/>
+      <c r="K141" s="2"/>
+      <c r="N141" s="3">
+        <v>6</v>
+      </c>
+      <c r="O141" s="3">
+        <v>14</v>
+      </c>
+      <c r="P141" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="Q141" s="3" t="str">
+        <f>CONCATENATE("public Element ", A141, " { get; private set; } // ",B141," - Atomic Number ", C141)</f>
+        <v>public Element Uup { get; private set; } // Ununpentium - Atomic Number 115</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>398</v>
+      </c>
+      <c r="B142" t="s">
+        <v>396</v>
+      </c>
+      <c r="C142">
+        <v>116</v>
+      </c>
+      <c r="D142" t="b">
+        <v>0</v>
+      </c>
+      <c r="E142" t="s">
+        <v>379</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="H142">
+        <v>0</v>
+      </c>
+      <c r="I142">
+        <v>0</v>
+      </c>
+      <c r="N142">
+        <v>6</v>
+      </c>
+      <c r="O142">
+        <v>15</v>
+      </c>
+      <c r="P142" t="s">
+        <v>409</v>
+      </c>
+      <c r="Q142" t="str">
+        <f>CONCATENATE("public Element ", A142, " { get; private set; } // ",B142," - Atomic Number ", C142)</f>
+        <v>public Element Lv { get; private set; } // Livermorium - Atomic Number 116</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="C143" s="3">
+        <v>116</v>
+      </c>
+      <c r="D143" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="F143" s="3">
+        <v>0</v>
+      </c>
+      <c r="G143" s="3">
+        <v>0</v>
+      </c>
+      <c r="H143" s="3">
+        <v>0</v>
+      </c>
+      <c r="I143" s="3">
+        <v>0</v>
+      </c>
+      <c r="J143" s="2"/>
+      <c r="K143" s="2"/>
+      <c r="N143" s="3">
+        <v>6</v>
+      </c>
+      <c r="O143" s="3">
+        <v>15</v>
+      </c>
+      <c r="P143" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="Q143" s="3" t="str">
+        <f>CONCATENATE("public Element ", A143, " { get; private set; } // ",B143," - Atomic Number ", C143)</f>
+        <v>public Element Uuh { get; private set; } // Ununhexium - Atomic Number 116</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>428</v>
+      </c>
+      <c r="B144" t="s">
+        <v>432</v>
+      </c>
+      <c r="C144">
+        <v>117</v>
+      </c>
+      <c r="D144" t="b">
+        <v>0</v>
+      </c>
+      <c r="E144" t="s">
+        <v>379</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
+        <v>0</v>
+      </c>
+      <c r="N144">
+        <v>6</v>
+      </c>
+      <c r="O144">
+        <v>16</v>
+      </c>
+      <c r="P144" t="s">
+        <v>409</v>
+      </c>
+      <c r="Q144" t="str">
+        <f>CONCATENATE("public Element ", A144, " { get; private set; } // ",B144," - Atomic Number ", C144)</f>
         <v>public Element Ts { get; private set; } // Tennessine - Atomic Number 117</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="145" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="C145" s="3">
+        <v>117</v>
+      </c>
+      <c r="D145" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="F145" s="3">
+        <v>0</v>
+      </c>
+      <c r="G145" s="3">
+        <v>0</v>
+      </c>
+      <c r="H145" s="3">
+        <v>0</v>
+      </c>
+      <c r="I145" s="3">
+        <v>0</v>
+      </c>
+      <c r="J145" s="2"/>
+      <c r="K145" s="2"/>
+      <c r="N145" s="3">
+        <v>6</v>
+      </c>
+      <c r="O145" s="3">
+        <v>16</v>
+      </c>
+      <c r="P145" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="Q145" s="3" t="str">
+        <f>CONCATENATE("public Element ", A145, " { get; private set; } // ",B145," - Atomic Number ", C145)</f>
+        <v>public Element Uus { get; private set; } // Ununseptium - Atomic Number 117</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>429</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B146" t="s">
         <v>433</v>
       </c>
-      <c r="C141">
+      <c r="C146">
         <v>118</v>
       </c>
-      <c r="D141" t="b">
-        <v>0</v>
-      </c>
-      <c r="E141" t="s">
+      <c r="D146" t="b">
+        <v>0</v>
+      </c>
+      <c r="E146" t="s">
         <v>379</v>
       </c>
-      <c r="F141">
-        <v>0</v>
-      </c>
-      <c r="G141">
-        <v>0</v>
-      </c>
-      <c r="H141">
-        <v>0</v>
-      </c>
-      <c r="I141">
-        <v>0</v>
-      </c>
-      <c r="N141">
+      <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+      <c r="I146">
+        <v>0</v>
+      </c>
+      <c r="N146">
         <v>6</v>
       </c>
-      <c r="O141">
+      <c r="O146">
         <v>17</v>
       </c>
-      <c r="P141" t="s">
+      <c r="P146" t="s">
         <v>409</v>
       </c>
-      <c r="Q141" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q146" t="str">
+        <f>CONCATENATE("public Element ", A146, " { get; private set; } // ",B146," - Atomic Number ", C146)</f>
         <v>public Element Og { get; private set; } // Oganesson - Atomic Number 118</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="C147" s="3">
+        <v>118</v>
+      </c>
+      <c r="D147" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="F147" s="3">
+        <v>0</v>
+      </c>
+      <c r="G147" s="3">
+        <v>0</v>
+      </c>
+      <c r="H147" s="3">
+        <v>0</v>
+      </c>
+      <c r="I147" s="3">
+        <v>0</v>
+      </c>
+      <c r="J147" s="2"/>
+      <c r="K147" s="2"/>
+      <c r="N147" s="3">
+        <v>6</v>
+      </c>
+      <c r="O147" s="3">
+        <v>17</v>
+      </c>
+      <c r="P147" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="Q147" s="3" t="str">
+        <f>CONCATENATE("public Element ", A147, " { get; private set; } // ",B147," - Atomic Number ", C147)</f>
+        <v>public Element Uuo { get; private set; } // Ununoctium - Atomic Number 118</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M141"/>
-  <sortState ref="A2:M141">
-    <sortCondition ref="A2:A141"/>
+  <sortState ref="A2:Q147">
+    <sortCondition ref="C2:C147"/>
+    <sortCondition ref="A2:A147"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>